<commit_message>
so pra dar merge
</commit_message>
<xml_diff>
--- a/Casa.xlsx
+++ b/Casa.xlsx
@@ -493,7 +493,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t xml:space="preserve">Bom </t>
+          <t>bom</t>
         </is>
       </c>
       <c r="E2" t="n">
@@ -513,15 +513,15 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Ruim</t>
+          <t>dia</t>
         </is>
       </c>
       <c r="E3" t="n">
-        <v>46</v>
+        <v>0</v>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>Vermelho</t>
+          <t>branca</t>
         </is>
       </c>
     </row>
@@ -536,7 +536,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H1"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -584,6 +584,29 @@
         <is>
           <t>Cor</t>
         </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Quarto</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Bom</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="D2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2" t="n">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Ar e lampada funcionando
sou foda
</commit_message>
<xml_diff>
--- a/Casa.xlsx
+++ b/Casa.xlsx
@@ -435,7 +435,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H6"/>
+  <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -488,100 +488,140 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Quarto</t>
+          <t>jo</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>lampada3</t>
         </is>
       </c>
       <c r="E2" t="n">
-        <v>0</v>
+        <v>48</v>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>branca</t>
+          <t>Azul</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Quarto</t>
+          <t>ji</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>pi</t>
         </is>
       </c>
       <c r="E3" t="n">
-        <v>0</v>
+        <v>59</v>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>branca</t>
+          <t>Vermelho</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Breno</t>
+          <t>ji</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>joia</t>
+          <t>po</t>
         </is>
       </c>
       <c r="E4" t="n">
-        <v>55</v>
+        <v>100</v>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>Azul</t>
+          <t>Branco</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Breno</t>
+          <t>jp</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>medio</t>
+          <t>dsakodas</t>
         </is>
       </c>
       <c r="E5" t="n">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>branca</t>
+          <t>Branco</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Breno</t>
+          <t>jp</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>ruim</t>
+          <t>vvcx</t>
         </is>
       </c>
       <c r="E6" t="n">
-        <v>60</v>
+        <v>78</v>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>Roxo</t>
+          <t>Verde</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>jo</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Bom dia</t>
+        </is>
+      </c>
+      <c r="E7" t="n">
+        <v>0</v>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>branca</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>ji</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>alo</t>
+        </is>
+      </c>
+      <c r="E8" t="n">
+        <v>0</v>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>branca</t>
         </is>
       </c>
     </row>
@@ -596,7 +636,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -649,12 +689,12 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Quarto</t>
+          <t>jo</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>bom dia</t>
+          <t>vai dar</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -663,21 +703,21 @@
         </is>
       </c>
       <c r="D2" t="n">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="E2" t="n">
-        <v>52</v>
+        <v>65</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Quarto</t>
+          <t>ji</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>dsdadsa</t>
+          <t>que bom</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -689,29 +729,6 @@
         <v>0</v>
       </c>
       <c r="E3" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>Breno</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>False</t>
-        </is>
-      </c>
-      <c r="D4" t="n">
-        <v>0</v>
-      </c>
-      <c r="E4" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Lampada e ar funcionadno de verdade agr
</commit_message>
<xml_diff>
--- a/Casa.xlsx
+++ b/Casa.xlsx
@@ -636,7 +636,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -702,11 +702,15 @@
           <t>True</t>
         </is>
       </c>
-      <c r="D2" t="n">
-        <v>14</v>
-      </c>
-      <c r="E2" t="n">
-        <v>65</v>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
       </c>
     </row>
     <row r="3">
@@ -729,6 +733,52 @@
         <v>0</v>
       </c>
       <c r="E3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>teste</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>teste</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
+        <v>0</v>
+      </c>
+      <c r="E4" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>ji</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>vai da corinthinas</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
+        <v>0</v>
+      </c>
+      <c r="E5" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
So falta cortina arrumado
</commit_message>
<xml_diff>
--- a/Casa.xlsx
+++ b/Casa.xlsx
@@ -496,7 +496,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -549,23 +549,138 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
+          <t>Bom</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Ar1</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="D2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Bom</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="D3" t="n">
+        <v>15</v>
+      </c>
+      <c r="E3" t="n">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Bom</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
+        <v>0</v>
+      </c>
+      <c r="E4" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
           <t>sorte</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>dasdsa</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
+        <v>13</v>
+      </c>
+      <c r="E5" t="n">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>sorte</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>23</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
         <is>
           <t>False</t>
         </is>
       </c>
-      <c r="D2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E2" t="n">
+      <c r="D6" t="n">
+        <v>0</v>
+      </c>
+      <c r="E6" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>sorte</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>4312</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
+        <v>0</v>
+      </c>
+      <c r="E7" t="n">
         <v>0</v>
       </c>
     </row>
@@ -580,7 +695,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H1"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -627,6 +742,66 @@
       <c r="H1" t="inlineStr">
         <is>
           <t>Cor</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>sorte</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>fdsoj</t>
+        </is>
+      </c>
+      <c r="F2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Bom</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="F3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>sorte</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="F4" t="n">
+        <v>0</v>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>False</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Acho q ta bom., falta testar
</commit_message>
<xml_diff>
--- a/Casa.xlsx
+++ b/Casa.xlsx
@@ -496,7 +496,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H7"/>
+  <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -546,144 +546,6 @@
         </is>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>Bom</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>Ar1</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>False</t>
-        </is>
-      </c>
-      <c r="D2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E2" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>Bom</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>True</t>
-        </is>
-      </c>
-      <c r="D3" t="n">
-        <v>15</v>
-      </c>
-      <c r="E3" t="n">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>Bom</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>False</t>
-        </is>
-      </c>
-      <c r="D4" t="n">
-        <v>0</v>
-      </c>
-      <c r="E4" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>sorte</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>True</t>
-        </is>
-      </c>
-      <c r="D5" t="n">
-        <v>13</v>
-      </c>
-      <c r="E5" t="n">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>sorte</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>23</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>False</t>
-        </is>
-      </c>
-      <c r="D6" t="n">
-        <v>0</v>
-      </c>
-      <c r="E6" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>sorte</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>4312</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>False</t>
-        </is>
-      </c>
-      <c r="D7" t="n">
-        <v>0</v>
-      </c>
-      <c r="E7" t="n">
-        <v>0</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -695,7 +557,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -742,66 +604,6 @@
       <c r="H1" t="inlineStr">
         <is>
           <t>Cor</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>sorte</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>fdsoj</t>
-        </is>
-      </c>
-      <c r="F2" t="n">
-        <v>0</v>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>True</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>Bom</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="F3" t="n">
-        <v>0</v>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>False</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>sorte</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="F4" t="n">
-        <v>0</v>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>False</t>
         </is>
       </c>
     </row>

</xml_diff>